<commit_message>
add code data for parquet data
</commit_message>
<xml_diff>
--- a/Team Mamoot/table schema.xlsx
+++ b/Team Mamoot/table schema.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="276">
   <si>
     <t>CODE</t>
   </si>
@@ -859,6 +859,41 @@
   </si>
   <si>
     <t>acftref</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 - Glider
+2 - Balloon
+3 - Blimp/Dirigible
+4 - Fixed wing single engine
+5 - Fixed wing multi engine
+6 - Rotorcraft
+7 - Weight-shift-control
+8 - Powered Parachute
+9 - Gyroplane</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0 - None
+1 - Reciprocating
+2 - Turbo-prop
+3 - Turbo-shaft
+4 - Turbo-jet
+5 - Turbo-fan
+6 - Ramjet
+7 - 2 Cycle
+8 - 4 Cycle
+9 – Unknown
+10 – Electric
+11 - Rotary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manufacturer Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MODEL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -926,7 +961,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -947,6 +982,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1252,7 +1293,7 @@
   <dimension ref="B1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1261,6 +1302,7 @@
     <col min="2" max="2" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.69921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.4">
@@ -1290,6 +1332,7 @@
       <c r="E2" s="6" t="s">
         <v>169</v>
       </c>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
@@ -1304,6 +1347,7 @@
       <c r="E3" s="3" t="s">
         <v>170</v>
       </c>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
@@ -1318,13 +1362,16 @@
       <c r="E4" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="F4" s="7" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>275</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
@@ -1332,8 +1379,9 @@
       <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:17" ht="156.6" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -1346,8 +1394,11 @@
       <c r="E6" s="3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="F6" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="208.8" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1359,6 +1410,9 @@
       </c>
       <c r="E7" s="3" t="s">
         <v>172</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.4">
@@ -1374,6 +1428,7 @@
       <c r="E8" s="3" t="s">
         <v>109</v>
       </c>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B9" s="2" t="s">
@@ -1388,6 +1443,7 @@
       <c r="E9" s="3" t="s">
         <v>109</v>
       </c>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B10" s="2" t="s">
@@ -1402,6 +1458,7 @@
       <c r="E10" s="3" t="s">
         <v>173</v>
       </c>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B11" s="2" t="s">
@@ -1416,6 +1473,7 @@
       <c r="E11" s="3" t="s">
         <v>144</v>
       </c>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B12" s="2" t="s">
@@ -1430,6 +1488,7 @@
       <c r="E12" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B13" s="2" t="s">
@@ -1444,6 +1503,7 @@
       <c r="E13" s="3" t="s">
         <v>174</v>
       </c>
+      <c r="F13" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>